<commit_message>
Integracion de la libreria DOMPDF y generacion de los pdf
</commit_message>
<xml_diff>
--- a/public/reportes/POAS.xlsx
+++ b/public/reportes/POAS.xlsx
@@ -89,11 +89,6 @@
           <t>Organismo</t>
         </is>
       </c>
-      <c r="B1" s="0" t="inlineStr">
-        <is>
-          <t>Secretaría de Finanzas</t>
-        </is>
-      </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="inlineStr">
@@ -101,11 +96,6 @@
           <t>Programa Presupuestario</t>
         </is>
       </c>
-      <c r="B2" s="0" t="inlineStr">
-        <is>
-          <t>Energía</t>
-        </is>
-      </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="inlineStr">
@@ -113,11 +103,6 @@
           <t>Clasificación Programatica (Grupo de Gasto)</t>
         </is>
       </c>
-      <c r="B3" s="0" t="inlineStr">
-        <is>
-          <t>Programable</t>
-        </is>
-      </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="inlineStr">
@@ -125,11 +110,6 @@
           <t>Clasificación Programatica (Grupo de Programa)</t>
         </is>
       </c>
-      <c r="B4" s="0" t="inlineStr">
-        <is>
-          <t>Desempeño de las Funciones</t>
-        </is>
-      </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="inlineStr">
@@ -137,11 +117,6 @@
           <t>Clasificación Programatica (Modalidad)</t>
         </is>
       </c>
-      <c r="B5" s="0" t="inlineStr">
-        <is>
-          <t>P - Planeación, formulación, implementación, seguimiento y evaluación de políticas públicas</t>
-        </is>
-      </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="inlineStr">
@@ -149,11 +124,6 @@
           <t>Gasto de orden</t>
         </is>
       </c>
-      <c r="B6" s="0" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="inlineStr">
@@ -202,7 +172,7 @@
       </c>
       <c r="B11" s="0" t="inlineStr">
         <is>
-          <t>07-05-2022 06:02:39 pm</t>
+          <t>07-07-2022 12:12:53 pm</t>
         </is>
       </c>
       <c r="E11" s="3" t="inlineStr">
@@ -256,40 +226,77 @@
     <row r="15" spans="1:8">
       <c r="A15" s="0" t="inlineStr">
         <is>
+          <t>Componente</t>
+        </is>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>6 Gobierno Ciudadano</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>5612</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>Sumatoria de POA alineados con el Plan Estatal de Desarrollo 2021-2027</t>
+        </is>
+      </c>
+      <c r="F15" s="0" t="inlineStr">
+        <is>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="G15" s="0" t="inlineStr">
+        <is>
+          <t>Mensual</t>
+        </is>
+      </c>
+      <c r="H15" s="0" t="inlineStr">
+        <is>
+          <t>Plan</t>
+        </is>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="0" t="inlineStr">
+        <is>
           <t>Fin</t>
         </is>
       </c>
-      <c r="B15" s="0" t="inlineStr">
+      <c r="B16" s="0" t="inlineStr">
         <is>
           <t>2.1 Aumento en el nivel educativo promedio de la población del estado. </t>
         </is>
       </c>
-      <c r="C15" s="0" t="inlineStr">
+      <c r="C16" s="0" t="inlineStr">
         <is>
           <t>5512</t>
         </is>
       </c>
-      <c r="D15" s="0" t="inlineStr">
+      <c r="D16" s="0" t="inlineStr">
         <is>
           <t>Porcentaje de Proyectos del Plan Querétaro Digital liberados con respecto al total de Proyectos</t>
         </is>
       </c>
-      <c r="E15" s="0" t="inlineStr">
+      <c r="E16" s="0" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="F15" s="0" t="inlineStr">
+      <c r="F16" s="0" t="inlineStr">
         <is>
           <t>80</t>
         </is>
       </c>
-      <c r="G15" s="0" t="inlineStr">
+      <c r="G16" s="0" t="inlineStr">
         <is>
           <t>Trimestral</t>
         </is>
       </c>
-      <c r="H15" s="0" t="inlineStr">
+      <c r="H16" s="0" t="inlineStr">
         <is>
           <t>Proyecto</t>
         </is>

</xml_diff>